<commit_message>
'Gust of Wind'final version
</commit_message>
<xml_diff>
--- a/finance/'Gust of Wind' balance sheet final version.xlsx
+++ b/finance/'Gust of Wind' balance sheet final version.xlsx
@@ -138,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="218">
   <si>
     <t>depreciation</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -865,9 +865,6 @@
   </si>
   <si>
     <t>BEP-week&amp;pallet</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
   <si>
     <t>vc per pallet</t>
@@ -1823,6 +1820,25 @@
     <xf numFmtId="169" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="9" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1847,25 +1863,6 @@
     <xf numFmtId="169" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="4" fillId="9" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="26">
     <cellStyle name="Comma" xfId="17" builtinId="3"/>
@@ -4395,13 +4392,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="139" t="s">
+      <c r="B1" s="146" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="140"/>
+      <c r="C1" s="147"/>
       <c r="D1" s="14"/>
-      <c r="E1" s="141"/>
-      <c r="F1" s="142"/>
+      <c r="E1" s="148"/>
+      <c r="F1" s="149"/>
       <c r="G1" s="89"/>
       <c r="H1" s="89"/>
       <c r="I1" s="89"/>
@@ -4430,15 +4427,15 @@
       <c r="J3" s="89"/>
     </row>
     <row r="4" spans="2:10" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="143" t="s">
+      <c r="B4" s="150" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="144"/>
+      <c r="C4" s="151"/>
       <c r="D4" s="103"/>
-      <c r="E4" s="141" t="s">
+      <c r="E4" s="148" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="142"/>
+      <c r="F4" s="149"/>
       <c r="G4" s="95"/>
       <c r="H4" s="95"/>
       <c r="I4" s="95"/>
@@ -4618,10 +4615,10 @@
       <c r="J11" s="89"/>
     </row>
     <row r="12" spans="2:10" s="6" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="145" t="s">
+      <c r="B12" s="152" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="146"/>
+      <c r="C12" s="153"/>
       <c r="D12" s="8"/>
       <c r="E12" s="106" t="s">
         <v>97</v>
@@ -5087,11 +5084,11 @@
     <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3" s="3"/>
-      <c r="C3" s="147">
+      <c r="C3" s="139">
         <f>70000*22</f>
         <v>1540000</v>
       </c>
-      <c r="D3" s="147">
+      <c r="D3" s="139">
         <f>15000*22</f>
         <v>330000</v>
       </c>
@@ -5119,7 +5116,7 @@
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="147">
+      <c r="C4" s="139">
         <f>SYD(C3,D3,E3,1)</f>
         <v>220000</v>
       </c>
@@ -5146,7 +5143,7 @@
       <c r="B5" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="147"/>
+      <c r="C5" s="139"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -5155,22 +5152,22 @@
     <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.25">
       <c r="A6" s="18"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="147">
+      <c r="C6" s="139">
         <f>70000*40</f>
         <v>2800000</v>
       </c>
-      <c r="D6" s="147">
+      <c r="D6" s="139">
         <f>15000*40</f>
         <v>600000</v>
       </c>
-      <c r="E6" s="147">
+      <c r="E6" s="139">
         <v>10</v>
       </c>
-      <c r="F6" s="147">
+      <c r="F6" s="139">
         <f>SYD($C$6,$D$6,$E$6,1)</f>
         <v>400000</v>
       </c>
-      <c r="G6" s="149">
+      <c r="G6" s="141">
         <f>SYD($C$6,$D$6,$E$6,2)</f>
         <v>360000</v>
       </c>
@@ -5189,13 +5186,13 @@
       <c r="B7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="147">
+      <c r="C7" s="139">
         <f>SYD($C$6,$D$6,$E$6,3)</f>
         <v>320000</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="147">
+      <c r="F7" s="139">
         <f>C6-F6-G6</f>
         <v>2040000</v>
       </c>
@@ -5237,11 +5234,11 @@
     <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="147">
+      <c r="C9" s="139">
         <f>70000*20</f>
         <v>1400000</v>
       </c>
-      <c r="D9" s="147">
+      <c r="D9" s="139">
         <f>15000*20</f>
         <v>300000</v>
       </c>
@@ -5266,7 +5263,7 @@
       <c r="B10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="147">
+      <c r="C10" s="139">
         <f>SYD($C$9,$D$9,$E$9,6)</f>
         <v>100000</v>
       </c>
@@ -5289,23 +5286,23 @@
     <row r="11" spans="1:12" ht="16" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="3"/>
-      <c r="C11" s="147">
+      <c r="C11" s="139">
         <f>SYD($C$9,$D$9,$E$9,1)</f>
         <v>200000</v>
       </c>
-      <c r="D11" s="147">
+      <c r="D11" s="139">
         <f>SYD($C$9,$D$9,$E$9,2)</f>
         <v>180000</v>
       </c>
-      <c r="E11" s="147">
+      <c r="E11" s="139">
         <f>SYD($C$9,$D$9,$E$9,3)</f>
         <v>160000</v>
       </c>
-      <c r="F11" s="147">
+      <c r="F11" s="139">
         <f>SYD($C$9,$D$9,$E$9,4)</f>
         <v>140000</v>
       </c>
-      <c r="G11" s="149">
+      <c r="G11" s="141">
         <f>SYD($C$9,$D$9,$E$9,5)</f>
         <v>120000</v>
       </c>
@@ -5326,7 +5323,7 @@
       <c r="C12" s="23"/>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
-      <c r="F12" s="150">
+      <c r="F12" s="142">
         <f>C9-SUM(C11:G11)</f>
         <v>600000</v>
       </c>
@@ -5385,7 +5382,7 @@
       <c r="B15" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="147">
+      <c r="C15" s="139">
         <v>20000</v>
       </c>
       <c r="D15" s="29">
@@ -5406,17 +5403,17 @@
       <c r="B16" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="147">
+      <c r="C16" s="139">
         <v>200000</v>
       </c>
-      <c r="D16" s="147">
+      <c r="D16" s="139">
         <v>30000</v>
       </c>
-      <c r="E16" s="147">
+      <c r="E16" s="139">
         <f>(C16-D16)/$D$14</f>
         <v>4250</v>
       </c>
-      <c r="F16" s="147">
+      <c r="F16" s="139">
         <f>C16-E16*D15</f>
         <v>157500</v>
       </c>
@@ -5435,7 +5432,7 @@
       <c r="B17" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="147">
+      <c r="C17" s="139">
         <f>55000*5</f>
         <v>275000</v>
       </c>
@@ -5448,7 +5445,7 @@
       <c r="B18" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="147">
+      <c r="C18" s="139">
         <v>25000</v>
       </c>
       <c r="D18" s="29">
@@ -5461,17 +5458,17 @@
       <c r="B19" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="147">
+      <c r="C19" s="139">
         <v>220000</v>
       </c>
-      <c r="D19" s="147">
+      <c r="D19" s="139">
         <v>36000</v>
       </c>
-      <c r="E19" s="147">
+      <c r="E19" s="139">
         <f>(C19-D19)/$D$14</f>
         <v>4600</v>
       </c>
-      <c r="F19" s="147">
+      <c r="F19" s="139">
         <f>C19-E19*D18</f>
         <v>164800</v>
       </c>
@@ -5482,7 +5479,7 @@
       <c r="B20" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="147">
+      <c r="C20" s="139">
         <f>55000*5</f>
         <v>275000</v>
       </c>
@@ -5495,7 +5492,7 @@
       <c r="B21" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="147">
+      <c r="C21" s="139">
         <v>40000</v>
       </c>
       <c r="D21" s="29">
@@ -5508,17 +5505,17 @@
       <c r="B22" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="147">
+      <c r="C22" s="139">
         <v>400000</v>
       </c>
-      <c r="D22" s="147">
+      <c r="D22" s="139">
         <v>90000</v>
       </c>
-      <c r="E22" s="147">
+      <c r="E22" s="139">
         <f>(C22-D22)/$D$14</f>
         <v>7750</v>
       </c>
-      <c r="F22" s="147">
+      <c r="F22" s="139">
         <f>C22-E22*D21</f>
         <v>183000</v>
       </c>
@@ -5529,11 +5526,11 @@
       <c r="B23" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="C23" s="150">
+      <c r="C23" s="142">
         <f>55000*7</f>
         <v>385000</v>
       </c>
-      <c r="D23" s="150"/>
+      <c r="D23" s="142"/>
       <c r="E23" s="32"/>
       <c r="F23" s="32"/>
       <c r="G23" s="33"/>
@@ -5552,10 +5549,10 @@
       <c r="A27" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="150">
+      <c r="B27" s="142">
         <v>100000</v>
       </c>
-      <c r="C27" s="151">
+      <c r="C27" s="143">
         <v>10</v>
       </c>
     </row>
@@ -5598,18 +5595,18 @@
         <v>62</v>
       </c>
       <c r="B31" s="3"/>
-      <c r="C31" s="147">
+      <c r="C31" s="139">
         <f>C17</f>
         <v>275000</v>
       </c>
-      <c r="D31" s="147">
+      <c r="D31" s="139">
         <f>5000*5</f>
         <v>25000</v>
       </c>
       <c r="E31" s="3">
         <v>30</v>
       </c>
-      <c r="F31" s="147">
+      <c r="F31" s="139">
         <f>C31-SUM(C33:L33)</f>
         <v>137903.22580645161</v>
       </c>
@@ -5659,47 +5656,47 @@
       <c r="B33" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C33" s="148">
+      <c r="C33" s="140">
         <f>SYD($C$31,$D$31,$E$31,1)</f>
         <v>16129.032258064517</v>
       </c>
-      <c r="D33" s="148">
+      <c r="D33" s="140">
         <f>SYD($C$31,$D$31,$E$31,2)</f>
         <v>15591.397849462366</v>
       </c>
-      <c r="E33" s="148">
+      <c r="E33" s="140">
         <f>SYD($C$31,$D$31,$E$31,3)</f>
         <v>15053.763440860215</v>
       </c>
-      <c r="F33" s="148">
+      <c r="F33" s="140">
         <f>SYD($C$31,$D$31,$E$31,4)</f>
         <v>14516.129032258064</v>
       </c>
-      <c r="G33" s="148">
+      <c r="G33" s="140">
         <f>SYD($C$31,$D$31,$E$31,5)</f>
         <v>13978.494623655914</v>
       </c>
-      <c r="H33" s="148">
+      <c r="H33" s="140">
         <f>SYD($C$31,$D$31,$E$31,6)</f>
         <v>13440.860215053763</v>
       </c>
-      <c r="I33" s="148">
+      <c r="I33" s="140">
         <f>SYD($C$31,$D$31,$E$31,7)</f>
         <v>12903.225806451614</v>
       </c>
-      <c r="J33" s="148">
+      <c r="J33" s="140">
         <f>SYD($C$31,$D$31,$E$31,8)</f>
         <v>12365.591397849463</v>
       </c>
-      <c r="K33" s="148">
+      <c r="K33" s="140">
         <f>SYD($C$31,$D$31,$E$31,9)</f>
         <v>11827.956989247312</v>
       </c>
-      <c r="L33" s="148">
+      <c r="L33" s="140">
         <f>SYD($C$31,$D$31,$E$31,10)</f>
         <v>11290.322580645161</v>
       </c>
-      <c r="M33" s="148">
+      <c r="M33" s="140">
         <f>SYD($C$31,$D$31,$E$31,11)</f>
         <v>10752.68817204301</v>
       </c>
@@ -5722,11 +5719,11 @@
         <v>63</v>
       </c>
       <c r="B35" s="3"/>
-      <c r="C35" s="147">
+      <c r="C35" s="139">
         <f>C20</f>
         <v>275000</v>
       </c>
-      <c r="D35" s="147">
+      <c r="D35" s="139">
         <f>5000*5</f>
         <v>25000</v>
       </c>
@@ -5788,55 +5785,55 @@
       <c r="B37" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C37" s="148">
+      <c r="C37" s="140">
         <f>SYD($C$35,$D$35,$E$35,1)</f>
         <v>16129.032258064517</v>
       </c>
-      <c r="D37" s="148">
+      <c r="D37" s="140">
         <f>SYD($C$35,$D$35,$E$35,2)</f>
         <v>15591.397849462366</v>
       </c>
-      <c r="E37" s="148">
+      <c r="E37" s="140">
         <f>SYD($C$35,$D$35,$E$35,3)</f>
         <v>15053.763440860215</v>
       </c>
-      <c r="F37" s="148">
+      <c r="F37" s="140">
         <f>SYD($C$35,$D$35,$E$35,4)</f>
         <v>14516.129032258064</v>
       </c>
-      <c r="G37" s="148">
+      <c r="G37" s="140">
         <f>SYD($C$35,$D$35,$E$35,5)</f>
         <v>13978.494623655914</v>
       </c>
-      <c r="H37" s="148">
+      <c r="H37" s="140">
         <f>SYD($C$35,$D$35,$E$35,6)</f>
         <v>13440.860215053763</v>
       </c>
-      <c r="I37" s="148">
+      <c r="I37" s="140">
         <f>SYD($C$35,$D$35,$E$35,7)</f>
         <v>12903.225806451614</v>
       </c>
-      <c r="J37" s="148">
+      <c r="J37" s="140">
         <f>SYD($C$35,$D$35,$E$35,8)</f>
         <v>12365.591397849463</v>
       </c>
-      <c r="K37" s="148">
+      <c r="K37" s="140">
         <f>SYD($C$35,$D$35,$E$35,9)</f>
         <v>11827.956989247312</v>
       </c>
-      <c r="L37" s="148">
+      <c r="L37" s="140">
         <f>SYD($C$35,$D$35,$E$35,10)</f>
         <v>11290.322580645161</v>
       </c>
-      <c r="M37" s="148">
+      <c r="M37" s="140">
         <f>SYD($C$35,$D$35,$E$35,11)</f>
         <v>10752.68817204301</v>
       </c>
-      <c r="N37" s="148">
+      <c r="N37" s="140">
         <f>SYD($C$35,$D$35,$E$35,12)</f>
         <v>10215.053763440861</v>
       </c>
-      <c r="O37" s="152">
+      <c r="O37" s="144">
         <f>SYD($C$35,$D$35,$E$35,13)</f>
         <v>9677.4193548387102</v>
       </c>
@@ -5858,18 +5855,18 @@
         <v>64</v>
       </c>
       <c r="B39" s="3"/>
-      <c r="C39" s="147">
+      <c r="C39" s="139">
         <f>C23</f>
         <v>385000</v>
       </c>
-      <c r="D39" s="147">
+      <c r="D39" s="139">
         <f>5000*7</f>
         <v>35000</v>
       </c>
       <c r="E39" s="3">
         <v>30</v>
       </c>
-      <c r="F39" s="147">
+      <c r="F39" s="139">
         <f>C39-SUM(C41:M41,C43:M43,C45:H45)</f>
         <v>37258.064516129205</v>
       </c>
@@ -5919,47 +5916,47 @@
       <c r="B41" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C41" s="148">
+      <c r="C41" s="140">
         <f>SYD($C$39,$D$39,$E$39,1)</f>
         <v>22580.645161290322</v>
       </c>
-      <c r="D41" s="148">
+      <c r="D41" s="140">
         <f>SYD($C$39,$D$39,$E$39,2)</f>
         <v>21827.956989247312</v>
       </c>
-      <c r="E41" s="148">
+      <c r="E41" s="140">
         <f>SYD($C$39,$D$39,$E$39,3)</f>
         <v>21075.268817204302</v>
       </c>
-      <c r="F41" s="148">
+      <c r="F41" s="140">
         <f>SYD($C$39,$D$39,$E$39,4)</f>
         <v>20322.580645161292</v>
       </c>
-      <c r="G41" s="148">
+      <c r="G41" s="140">
         <f>SYD($C$39,$D$39,$E$39,5)</f>
         <v>19569.892473118278</v>
       </c>
-      <c r="H41" s="148">
+      <c r="H41" s="140">
         <f>SYD($C$39,$D$39,$E$39,6)</f>
         <v>18817.204301075268</v>
       </c>
-      <c r="I41" s="148">
+      <c r="I41" s="140">
         <f>SYD($C$39,$D$39,$E$39,7)</f>
         <v>18064.516129032258</v>
       </c>
-      <c r="J41" s="148">
+      <c r="J41" s="140">
         <f>SYD($C$39,$D$39,$E$39,8)</f>
         <v>17311.827956989247</v>
       </c>
-      <c r="K41" s="148">
+      <c r="K41" s="140">
         <f>SYD($C$39,$D$39,$E$39,9)</f>
         <v>16559.139784946237</v>
       </c>
-      <c r="L41" s="148">
+      <c r="L41" s="140">
         <f>SYD($C$39,$D$39,$E$39,10)</f>
         <v>15806.451612903225</v>
       </c>
-      <c r="M41" s="148">
+      <c r="M41" s="140">
         <f>SYD($C$39,$D$39,$E$39,11)</f>
         <v>15053.763440860215</v>
       </c>
@@ -6004,47 +6001,47 @@
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A43" s="28"/>
-      <c r="C43" s="148">
+      <c r="C43" s="140">
         <f>SYD($C$39,$D$39,$E$39,12)</f>
         <v>14301.075268817205</v>
       </c>
-      <c r="D43" s="148">
+      <c r="D43" s="140">
         <f>SYD($C$39,$D$39,$E$39,13)</f>
         <v>13548.387096774193</v>
       </c>
-      <c r="E43" s="148">
+      <c r="E43" s="140">
         <f>SYD($C$39,$D$39,$E$39,14)</f>
         <v>12795.698924731183</v>
       </c>
-      <c r="F43" s="148">
+      <c r="F43" s="140">
         <f>SYD($C$39,$D$39,$E$39,15)</f>
         <v>12043.010752688173</v>
       </c>
-      <c r="G43" s="148">
+      <c r="G43" s="140">
         <f>SYD($C$39,$D$39,$E$39,16)</f>
         <v>11290.322580645161</v>
       </c>
-      <c r="H43" s="148">
+      <c r="H43" s="140">
         <f>SYD($C$39,$D$39,$E$39,17)</f>
         <v>10537.634408602151</v>
       </c>
-      <c r="I43" s="148">
+      <c r="I43" s="140">
         <f>SYD($C$39,$D$39,$E$39,18)</f>
         <v>9784.9462365591389</v>
       </c>
-      <c r="J43" s="148">
+      <c r="J43" s="140">
         <f>SYD($C$39,$D$39,$E$39,19)</f>
         <v>9032.2580645161288</v>
       </c>
-      <c r="K43" s="148">
+      <c r="K43" s="140">
         <f>SYD($C$39,$D$39,$E$39,20)</f>
         <v>8279.5698924731187</v>
       </c>
-      <c r="L43" s="148">
+      <c r="L43" s="140">
         <f>SYD($C$39,$D$39,$E$39,21)</f>
         <v>7526.8817204301076</v>
       </c>
-      <c r="M43" s="148">
+      <c r="M43" s="140">
         <f>SYD($C$39,$D$39,$E$39,22)</f>
         <v>6774.1935483870966</v>
       </c>
@@ -6077,31 +6074,31 @@
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A45" s="28"/>
-      <c r="C45" s="148">
+      <c r="C45" s="140">
         <f>SYD($C$39,$D$39,$E$39,23)</f>
         <v>6021.5053763440865</v>
       </c>
-      <c r="D45" s="148">
+      <c r="D45" s="140">
         <f>SYD($C$39,$D$39,$E$39,24)</f>
         <v>5268.8172043010754</v>
       </c>
-      <c r="E45" s="148">
+      <c r="E45" s="140">
         <f>SYD($C$39,$D$39,$E$39,25)</f>
         <v>4516.1290322580644</v>
       </c>
-      <c r="F45" s="148">
+      <c r="F45" s="140">
         <f>SYD($C$39,$D$39,$E$39,26)</f>
         <v>3763.4408602150538</v>
       </c>
-      <c r="G45" s="148">
+      <c r="G45" s="140">
         <f>SYD($C$39,$D$39,$E$39,27)</f>
         <v>3010.7526881720432</v>
       </c>
-      <c r="H45" s="148">
+      <c r="H45" s="140">
         <f>SYD($C$39,$D$39,$E$39,28)</f>
         <v>2258.0645161290322</v>
       </c>
-      <c r="I45" s="148">
+      <c r="I45" s="140">
         <f>SYD($C$39,$D$39,$E$39,29)</f>
         <v>1505.3763440860216</v>
       </c>
@@ -6135,7 +6132,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6159,7 +6156,7 @@
         <v>104000</v>
       </c>
       <c r="G1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H1" s="113">
         <f>SUM(E8:E22)</f>
@@ -6205,7 +6202,7 @@
         <v>24</v>
       </c>
       <c r="G4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H4" s="113">
         <f>B2</f>
@@ -6226,7 +6223,7 @@
       <c r="G6" t="s">
         <v>211</v>
       </c>
-      <c r="H6" s="153">
+      <c r="H6" s="145">
         <f>ROUNDUP(H2/(H4-H3),0)</f>
         <v>1213</v>
       </c>
@@ -6242,18 +6239,18 @@
         <v>207</v>
       </c>
       <c r="D7" t="s">
+        <v>212</v>
+      </c>
+      <c r="E7" t="s">
         <v>213</v>
-      </c>
-      <c r="E7" t="s">
-        <v>214</v>
       </c>
       <c r="F7" t="s">
         <v>209</v>
       </c>
       <c r="G7" t="s">
-        <v>215</v>
-      </c>
-      <c r="H7" s="153">
+        <v>214</v>
+      </c>
+      <c r="H7" s="145">
         <f>ROUNDUP(H1/(H4-H3),0)</f>
         <v>63073</v>
       </c>
@@ -6269,9 +6266,7 @@
         <f>-VLOOKUP(A8,'9-11'!H:I,2,0)</f>
         <v>1344000</v>
       </c>
-      <c r="D8" s="113" t="s">
-        <v>212</v>
-      </c>
+      <c r="D8" s="113"/>
       <c r="E8" s="113">
         <f>C8</f>
         <v>1344000</v>
@@ -6292,9 +6287,7 @@
         <f>-VLOOKUP(A9,'9-11'!H:I,2,0)+'9-11'!F8</f>
         <v>4368000</v>
       </c>
-      <c r="D9" s="113" t="s">
-        <v>212</v>
-      </c>
+      <c r="D9" s="113"/>
       <c r="E9" s="113">
         <f>C9</f>
         <v>4368000</v>
@@ -6315,9 +6308,7 @@
         <f>-VLOOKUP(A10,'9-11'!H:I,2,0)+'9-11'!F9</f>
         <v>262080</v>
       </c>
-      <c r="D10" s="113" t="s">
-        <v>212</v>
-      </c>
+      <c r="D10" s="113"/>
       <c r="E10" s="113">
         <f>C10</f>
         <v>262080</v>
@@ -6342,12 +6333,8 @@
         <f>C11/$B$1</f>
         <v>0.74045971153846146</v>
       </c>
-      <c r="E11" s="113" t="s">
-        <v>212</v>
-      </c>
-      <c r="F11" s="113" t="s">
-        <v>212</v>
-      </c>
+      <c r="E11" s="113"/>
+      <c r="F11" s="113"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12" s="107" t="s">
@@ -6364,12 +6351,8 @@
         <f>C12/$B$1</f>
         <v>1.4807692307692308</v>
       </c>
-      <c r="E12" s="113" t="s">
-        <v>212</v>
-      </c>
-      <c r="F12" s="113" t="s">
-        <v>212</v>
-      </c>
+      <c r="E12" s="113"/>
+      <c r="F12" s="113"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A13" s="107" t="s">
@@ -6382,9 +6365,7 @@
         <f>-VLOOKUP(A13,'9-11'!H:I,2,0)</f>
         <v>76870.661999999997</v>
       </c>
-      <c r="D13" s="113" t="s">
-        <v>212</v>
-      </c>
+      <c r="D13" s="113"/>
       <c r="E13" s="113">
         <f>C13</f>
         <v>76870.661999999997</v>
@@ -6405,9 +6386,7 @@
         <f>-VLOOKUP(A14,'9-11'!H:I,2,0)</f>
         <v>201600</v>
       </c>
-      <c r="D14" s="113" t="s">
-        <v>212</v>
-      </c>
+      <c r="D14" s="113"/>
       <c r="E14" s="113">
         <f>C14</f>
         <v>201600</v>
@@ -6432,12 +6411,8 @@
         <f>C15/$B$1</f>
         <v>25.96153846153846</v>
       </c>
-      <c r="E15" s="113" t="s">
-        <v>212</v>
-      </c>
-      <c r="F15" s="113" t="s">
-        <v>212</v>
-      </c>
+      <c r="E15" s="113"/>
+      <c r="F15" s="113"/>
     </row>
     <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.15">
       <c r="A16" s="95" t="s">
@@ -6450,9 +6425,7 @@
         <f>-VLOOKUP(A16,'9-11'!H:I,2,0)</f>
         <v>672000</v>
       </c>
-      <c r="D16" s="113" t="s">
-        <v>212</v>
-      </c>
+      <c r="D16" s="113"/>
       <c r="E16" s="113">
         <f>C16</f>
         <v>672000</v>
@@ -6477,12 +6450,8 @@
         <f>C17/$B$1</f>
         <v>16.900399144540941</v>
       </c>
-      <c r="E17" s="113" t="s">
-        <v>212</v>
-      </c>
-      <c r="F17" s="113" t="s">
-        <v>212</v>
-      </c>
+      <c r="E17" s="113"/>
+      <c r="F17" s="113"/>
     </row>
     <row r="18" spans="1:10" ht="16" x14ac:dyDescent="0.15">
       <c r="A18" s="95" t="s">
@@ -6495,9 +6464,7 @@
         <f>'9-11'!F11</f>
         <v>226300</v>
       </c>
-      <c r="D18" s="113" t="s">
-        <v>212</v>
-      </c>
+      <c r="D18" s="113"/>
       <c r="E18" s="113">
         <f>C18</f>
         <v>226300</v>
@@ -6507,7 +6474,7 @@
         <v>4351.9230769230771</v>
       </c>
       <c r="J18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16" x14ac:dyDescent="0.15">
@@ -6521,9 +6488,7 @@
         <f>'9-11'!F13</f>
         <v>885</v>
       </c>
-      <c r="D19" s="113" t="s">
-        <v>212</v>
-      </c>
+      <c r="D19" s="113"/>
       <c r="E19" s="113">
         <f>C19</f>
         <v>885</v>
@@ -6544,9 +6509,7 @@
         <f>-VLOOKUP(A20,'9-11'!H:I,2,0)</f>
         <v>640000</v>
       </c>
-      <c r="D20" s="113" t="s">
-        <v>212</v>
-      </c>
+      <c r="D20" s="113"/>
       <c r="E20" s="113">
         <f>C20</f>
         <v>640000</v>
@@ -6567,9 +6530,7 @@
         <f>-VLOOKUP(A21,'9-11'!H:I,2,0)</f>
         <v>16600</v>
       </c>
-      <c r="D21" s="113" t="s">
-        <v>212</v>
-      </c>
+      <c r="D21" s="113"/>
       <c r="E21" s="113">
         <f>C21</f>
         <v>16600</v>
@@ -6590,9 +6551,7 @@
         <f>-VLOOKUP(A22,'9-11'!H:I,2,0)</f>
         <v>21935.483870967742</v>
       </c>
-      <c r="D22" s="113" t="s">
-        <v>212</v>
-      </c>
+      <c r="D22" s="113"/>
       <c r="E22" s="113">
         <f>C22</f>
         <v>21935.483870967742</v>
@@ -7246,8 +7205,12 @@
           <x14:colorLow theme="3"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Income!D7:O7</xm:f>
-              <xm:sqref>C7</xm:sqref>
+              <xm:f>Income!$D$5:$O$5</xm:f>
+              <xm:sqref>C5</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Income!$D$6:$O$6</xm:f>
+              <xm:sqref>C6</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -7262,12 +7225,8 @@
           <x14:colorLow theme="3"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Income!$D$5:$O$5</xm:f>
-              <xm:sqref>C5</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Income!$D$6:$O$6</xm:f>
-              <xm:sqref>C6</xm:sqref>
+              <xm:f>Income!D7:O7</xm:f>
+              <xm:sqref>C7</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -9726,6 +9685,22 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup manualMax="0" manualMin="0" lineWeight="1" displayEmptyCellsAs="gap" high="1" low="1">
+          <x14:colorSeries theme="3"/>
+          <x14:colorNegative theme="5"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers theme="4" tint="-0.499984740745262"/>
+          <x14:colorFirst theme="4" tint="0.39997558519241921"/>
+          <x14:colorLast theme="4" tint="0.39997558519241921"/>
+          <x14:colorHigh theme="3"/>
+          <x14:colorLow theme="3"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Expenses!D24:O24</xm:f>
+              <xm:sqref>C24</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
         <x14:sparklineGroup manualMax="0" manualMin="0" lineWeight="1" displayEmptyCellsAs="gap" high="1" low="1">
           <x14:colorSeries theme="3"/>
           <x14:colorNegative theme="5"/>
@@ -9814,22 +9789,6 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup manualMax="0" manualMin="0" lineWeight="1" displayEmptyCellsAs="gap" high="1" low="1">
-          <x14:colorSeries theme="3"/>
-          <x14:colorNegative theme="5"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers theme="4" tint="-0.499984740745262"/>
-          <x14:colorFirst theme="4" tint="0.39997558519241921"/>
-          <x14:colorLast theme="4" tint="0.39997558519241921"/>
-          <x14:colorHigh theme="3"/>
-          <x14:colorLow theme="3"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>Expenses!D24:O24</xm:f>
-              <xm:sqref>C24</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
       </x14:sparklineGroups>
     </ext>
   </extLst>

</xml_diff>